<commit_message>
adding modified files-Test case file,Test Data files and TestNG.xml
</commit_message>
<xml_diff>
--- a/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
+++ b/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESA407961\workspace\ZYCUS\src\main\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESA407961\workspace\ZYCUS\startup\dev\ZYCUS\src\main\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>201</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Test Data</t>
-  </si>
-  <si>
-    <t>Expected HTTPS Code</t>
-  </si>
-  <si>
-    <t>Expected HTTPS Message/Body</t>
   </si>
   <si>
     <t>401</t>
@@ -118,15 +112,40 @@
   <si>
     <t>Test Step</t>
   </si>
+  <si>
+    <t>customerCreationInValidCustomerName.json</t>
+  </si>
+  <si>
+    <t>customerCreationInValidEmail.json</t>
+  </si>
+  <si>
+    <t>customerCreationInValidMobileNum.json</t>
+  </si>
+  <si>
+    <t>customerCreationValid.json</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Code&lt;TBD&gt;</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Message/Body&lt;TBD&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -177,6 +196,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +538,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -548,28 +568,28 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -577,16 +597,16 @@
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
@@ -597,16 +617,16 @@
     </row>
     <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>1</v>
@@ -617,16 +637,16 @@
     </row>
     <row r="5" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>1</v>
@@ -637,19 +657,19 @@
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -657,41 +677,36 @@
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4">
         <v>200</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>

</xml_diff>

<commit_message>
adding report generator, retry generator and core functionalities package
</commit_message>
<xml_diff>
--- a/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
+++ b/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>201</t>
   </si>
@@ -30,9 +30,6 @@
     <t>400</t>
   </si>
   <si>
-    <t>userCreationValid.json</t>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
@@ -46,15 +43,6 @@
   </si>
   <si>
     <t>401</t>
-  </si>
-  <si>
-    <t>Test Scenario_001: Get User By ID</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>Verify user can get customer details by providing valid customer id - GET/customer/&lt;ValidID&gt;</t>
   </si>
   <si>
     <t>Verify user is Not allowed to create new customer id with Invalid data:
@@ -95,40 +83,37 @@
     <t>Verify if Unautorized user is trying to create the new customer, 401 -Unauthorized is fired.</t>
   </si>
   <si>
-    <t>Verify user is displayed with 404 not found error if he provides invalid customerID in GET/customer/&lt;ValidID&gt;</t>
-  </si>
-  <si>
     <t>customers</t>
   </si>
   <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Test Step</t>
+  </si>
+  <si>
+    <t>customerCreationInValidCustomerName.json</t>
+  </si>
+  <si>
+    <t>customerCreationInValidEmail.json</t>
+  </si>
+  <si>
+    <t>customerCreationInValidMobileNum.json</t>
+  </si>
+  <si>
+    <t>customerCreationValid.json</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Code&lt;TBD&gt;</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Message/Body&lt;TBD&gt;</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
     <t>customers/ID</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>Test Step</t>
-  </si>
-  <si>
-    <t>customerCreationInValidCustomerName.json</t>
-  </si>
-  <si>
-    <t>customerCreationInValidEmail.json</t>
-  </si>
-  <si>
-    <t>customerCreationInValidMobileNum.json</t>
-  </si>
-  <si>
-    <t>customerCreationValid.json</t>
-  </si>
-  <si>
-    <t>Expected HTTPS Code&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Expected HTTPS Message/Body&lt;TBD&gt;</t>
   </si>
 </sst>
 </file>
@@ -186,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -196,7 +181,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,210 +539,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>28</v>
+      <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="4">
-        <v>200</v>
-      </c>
+      <c r="F7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding post,get core fuctions,class for saving customerid, classand completed the test case drafting in Zycus-Assignment.xlsx sheet
</commit_message>
<xml_diff>
--- a/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
+++ b/dev/ZYCUS/src/main/TestData/Zycus-Assignment.xlsx
@@ -22,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Test Case</t>
   </si>
@@ -40,9 +34,6 @@
   </si>
   <si>
     <t>Test Data</t>
-  </si>
-  <si>
-    <t>401</t>
   </si>
   <si>
     <t>Verify user is Not allowed to create new customer id with Invalid data:
@@ -104,16 +95,90 @@
     <t>customerCreationValid.json</t>
   </si>
   <si>
-    <t>Expected HTTPS Code&lt;TBD&gt;</t>
-  </si>
-  <si>
-    <t>Expected HTTPS Message/Body&lt;TBD&gt;</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
     <t>customers/ID</t>
+  </si>
+  <si>
+    <t>{
+  "HttpsStatusCode": "201",
+  "HttpsStatusInfo": "Created"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "HttpsStatusCode": "400",
+  "HttpsStatusInfo": "Bad Request"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "HttpsStatusCode": "401",
+  "HttpsStatusInfo": "Unauthorized"
+}</t>
+  </si>
+  <si>
+    <t>Test Scenario_001: Get User By ID</t>
+  </si>
+  <si>
+    <t>Verify user can get customer details by providing valid customer id - GET/customer/&lt;ValidID&gt;</t>
+  </si>
+  <si>
+    <t>Verify user is displayed with 404 not found error if he provides invalid customerID in GET/customer/&lt;ValidID&gt;</t>
+  </si>
+  <si>
+    <t>{
+  "HttpsStatusCode": "404",
+  "HttpsStatusInfo": "Not Found"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "HttpsStatusCode": "200",
+  "HttpsStatusInfo": "Ok"
+}</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Code</t>
+  </si>
+  <si>
+    <t>Expected HTTPS Entity Message/Body</t>
+  </si>
+  <si>
+    <t>{
+  "customerstatus": "active"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "code": "FUNC_006",
+  "message": "The request could not be completed due to Invalid Customer Name"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "code": "FUNC_007",
+  "message": "The request could not be completed due to Invalid Customer email id"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "code": "FUNC_008",
+  "message": "The request could not be completed due to Invalid Customer mobile number"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "code": "FUNC_008",
+  "message": "Unauthorized Attempt"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "code": "FUNC_009",
+  "message": "User id not found"
+}</t>
   </si>
 </sst>
 </file>
@@ -171,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -183,6 +248,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,178 +601,184 @@
     <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>

</xml_diff>